<commit_message>
Created Animation (utility) class with start and stop methods
</commit_message>
<xml_diff>
--- a/SolarSystem/data/Data.xlsx
+++ b/SolarSystem/data/Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Velmond\Desktop\solar-system-textures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvayloBotusharov\Dropbox\Ivo\IT\Telerik Academy\Telerik Academy 2013 (JS Part 2 Teamwork)\SolarSystem\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -848,6 +848,27 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -864,27 +885,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1169,8 +1169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Y20" sqref="Y20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,37 +1254,37 @@
       <c r="A2" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="84" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="78"/>
-      <c r="D2" s="79" t="s">
+      <c r="C2" s="85"/>
+      <c r="D2" s="86" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="80"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="79" t="s">
+      <c r="E2" s="87"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="86" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="80"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="79" t="s">
+      <c r="H2" s="87"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="86" t="s">
         <v>40</v>
       </c>
-      <c r="K2" s="80"/>
-      <c r="L2" s="81"/>
-      <c r="M2" s="87" t="s">
+      <c r="K2" s="87"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="N2" s="85"/>
-      <c r="O2" s="85" t="s">
+      <c r="N2" s="80"/>
+      <c r="O2" s="80" t="s">
         <v>42</v>
       </c>
-      <c r="P2" s="86"/>
-      <c r="Q2" s="83" t="s">
+      <c r="P2" s="81"/>
+      <c r="Q2" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="84"/>
+      <c r="R2" s="79"/>
       <c r="S2" s="13" t="s">
         <v>22</v>
       </c>
@@ -1991,20 +1991,20 @@
       <c r="C14" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="82" t="s">
+      <c r="D14" s="89" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="82"/>
+      <c r="E14" s="89"/>
       <c r="F14" s="76">
         <f>O6</f>
         <v>10000</v>
       </c>
-      <c r="H14" s="88" t="s">
+      <c r="H14" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="I14" s="88"/>
-      <c r="J14" s="88"/>
-      <c r="K14" s="88"/>
+      <c r="I14" s="83"/>
+      <c r="J14" s="83"/>
+      <c r="K14" s="83"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="38" t="s">
@@ -2017,19 +2017,19 @@
       <c r="C15" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="89" t="s">
+      <c r="D15" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="89"/>
+      <c r="E15" s="77"/>
       <c r="F15" s="1">
         <v>100</v>
       </c>
-      <c r="H15" s="88" t="s">
+      <c r="H15" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="I15" s="88"/>
-      <c r="J15" s="88"/>
-      <c r="K15" s="88"/>
+      <c r="I15" s="83"/>
+      <c r="J15" s="83"/>
+      <c r="K15" s="83"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="38" t="s">
@@ -2045,12 +2045,12 @@
       <c r="F16" s="1">
         <v>240</v>
       </c>
-      <c r="H16" s="88" t="s">
+      <c r="H16" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="I16" s="88"/>
-      <c r="J16" s="88"/>
-      <c r="K16" s="88"/>
+      <c r="I16" s="83"/>
+      <c r="J16" s="83"/>
+      <c r="K16" s="83"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="38" t="s">
@@ -2063,12 +2063,12 @@
       <c r="C17" t="s">
         <v>32</v>
       </c>
-      <c r="H17" s="88" t="s">
+      <c r="H17" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="I17" s="88"/>
-      <c r="J17" s="88"/>
-      <c r="K17" s="88"/>
+      <c r="I17" s="83"/>
+      <c r="J17" s="83"/>
+      <c r="K17" s="83"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="30"/>
@@ -2105,6 +2105,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="D14:E14"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="O2:P2"/>
@@ -2113,13 +2118,8 @@
     <mergeCell ref="H16:K16"/>
     <mergeCell ref="H15:K15"/>
     <mergeCell ref="H14:K14"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="D14:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="45" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed angular and orbital speed in data.js.
I had calculated the angular and orbital speeds wrong. Fixed them.
Fixed the unreadable comments in loader.js... Git clearly does not like
Cyrillic.
In the "data" folder -> Fixed the incorrect data in the excel file.
dataTest.js is almost the same as main.js but with the data from
data.js. This is how the animation would look like with the properties
in data.js.
Also with the new values for angular speed there is no need to divide by
1000 when calculating angleDiff at the end of main/dataTest (rows 425,
430 in main.js or 430, 435 in dataTest.js).
</commit_message>
<xml_diff>
--- a/SolarSystem/data/Data.xlsx
+++ b/SolarSystem/data/Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvayloBotusharov\Dropbox\Ivo\IT\Telerik Academy\Telerik Academy 2013 (JS Part 2 Teamwork)\SolarSystem\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Velmond\Desktop\SolarSystem\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -140,52 +140,53 @@
 Earth days</t>
   </si>
   <si>
+    <t>nPeriod</t>
+  </si>
+  <si>
+    <t>radius</t>
+  </si>
+  <si>
+    <t>orbitRadius</t>
+  </si>
+  <si>
+    <t>orbitRadiusX</t>
+  </si>
+  <si>
+    <t>orbitRadiusY</t>
+  </si>
+  <si>
+    <t>orbitSpeed</t>
+  </si>
+  <si>
+    <t>10000/orbitSpeed</t>
+  </si>
+  <si>
+    <t>angularSpeed</t>
+  </si>
+  <si>
+    <t>reduced?</t>
+  </si>
+  <si>
+    <t>10^6 km</t>
+  </si>
+  <si>
+    <t>Base period =</t>
+  </si>
+  <si>
+    <t>Speed factor =</t>
+  </si>
+  <si>
     <t>Period
-10000/TOS</t>
-  </si>
-  <si>
-    <t>nPeriod</t>
-  </si>
-  <si>
-    <t>radius</t>
-  </si>
-  <si>
-    <t>orbitRadius</t>
-  </si>
-  <si>
-    <t>orbitRadiusX</t>
-  </si>
-  <si>
-    <t>orbitRadiusY</t>
-  </si>
-  <si>
-    <t>orbitSpeed</t>
-  </si>
-  <si>
-    <t>10000/orbitSpeed</t>
-  </si>
-  <si>
-    <t>angularSpeed</t>
-  </si>
-  <si>
-    <t>reduced?</t>
-  </si>
-  <si>
-    <t>10^6 km</t>
-  </si>
-  <si>
-    <t>Base period =</t>
-  </si>
-  <si>
-    <t>Speed factor =</t>
+10k/TOS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -708,7 +709,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -817,20 +818,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -848,45 +835,67 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1169,8 +1178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W21"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Y20" sqref="Y20"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1208,7 +1217,7 @@
         <v>16</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G1" s="16" t="s">
         <v>15</v>
@@ -1217,7 +1226,7 @@
         <v>18</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J1" s="16" t="s">
         <v>14</v>
@@ -1226,19 +1235,19 @@
         <v>17</v>
       </c>
       <c r="L1" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M1" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="69" t="s">
+      <c r="N1" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="70" t="s">
+      <c r="O1" s="60" t="s">
+        <v>47</v>
+      </c>
+      <c r="P1" s="28" t="s">
         <v>35</v>
-      </c>
-      <c r="P1" s="28" t="s">
-        <v>36</v>
       </c>
       <c r="Q1" s="46" t="s">
         <v>34</v>
@@ -1254,37 +1263,37 @@
       <c r="A2" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="88" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="89"/>
+      <c r="D2" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="86" t="s">
+      <c r="E2" s="86"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="87"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="86" t="s">
+      <c r="H2" s="86"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="85" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="87"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="86" t="s">
+      <c r="K2" s="86"/>
+      <c r="L2" s="87"/>
+      <c r="M2" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="K2" s="87"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="82" t="s">
+      <c r="N2" s="84"/>
+      <c r="O2" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="N2" s="80"/>
-      <c r="O2" s="80" t="s">
+      <c r="P2" s="70"/>
+      <c r="Q2" s="81" t="s">
         <v>42</v>
       </c>
-      <c r="P2" s="81"/>
-      <c r="Q2" s="78" t="s">
-        <v>43</v>
-      </c>
-      <c r="R2" s="79"/>
+      <c r="R2" s="82"/>
       <c r="S2" s="13" t="s">
         <v>22</v>
       </c>
@@ -1330,23 +1339,23 @@
       <c r="M3" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="59">
+      <c r="N3" s="90">
         <f>10000/O3</f>
+        <v>1</v>
+      </c>
+      <c r="O3" s="91">
         <v>10000</v>
       </c>
-      <c r="O3" s="60">
+      <c r="P3" s="8">
+        <f>O3/$F$14</f>
         <v>1</v>
-      </c>
-      <c r="P3" s="8">
-        <f>O3/$F$14 *100</f>
-        <v>0.01</v>
       </c>
       <c r="Q3" s="45">
         <v>34</v>
       </c>
-      <c r="R3" s="24">
-        <f t="shared" ref="R3:R12" si="0">Q3/$B$17</f>
-        <v>34</v>
+      <c r="R3" s="72">
+        <f>$B$17/Q3</f>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="S3" s="54" t="s">
         <v>20</v>
@@ -1360,61 +1369,61 @@
         <v>2440</v>
       </c>
       <c r="C4" s="20">
-        <f t="shared" ref="C4:C12" si="1">B4/$B$15</f>
+        <f t="shared" ref="C4:C12" si="0">B4/$B$15</f>
         <v>0.38256506741925367</v>
       </c>
       <c r="D4" s="21">
-        <f t="shared" ref="D4:D12" si="2">(J4+G4)/2</f>
+        <f t="shared" ref="D4:D12" si="1">(J4+G4)/2</f>
         <v>58</v>
       </c>
-      <c r="E4" s="72">
-        <f t="shared" ref="E4:E12" si="3">D4/$B$14</f>
+      <c r="E4" s="62">
+        <f t="shared" ref="E4:E12" si="2">D4/$B$14</f>
         <v>0.38795986622073581</v>
       </c>
-      <c r="F4" s="73" t="s">
+      <c r="F4" s="63" t="s">
         <v>22</v>
       </c>
       <c r="G4" s="27">
         <v>70</v>
       </c>
       <c r="H4" s="47">
-        <f t="shared" ref="H4:H12" si="4">G4/$B$14</f>
+        <f t="shared" ref="H4:H12" si="3">G4/$B$14</f>
         <v>0.4682274247491639</v>
       </c>
-      <c r="I4" s="73" t="s">
+      <c r="I4" s="63" t="s">
         <v>22</v>
       </c>
       <c r="J4" s="27">
         <v>46</v>
       </c>
       <c r="K4" s="47">
-        <f t="shared" ref="K4:K12" si="5">J4/$B$14</f>
+        <f t="shared" ref="K4:K12" si="4">J4/$B$14</f>
         <v>0.30769230769230771</v>
       </c>
-      <c r="L4" s="73" t="s">
+      <c r="L4" s="63" t="s">
         <v>22</v>
       </c>
       <c r="M4" s="27">
         <v>88</v>
       </c>
-      <c r="N4" s="61">
-        <f t="shared" ref="N4:N12" si="6">M4/$B$16</f>
-        <v>0.24096385542168675</v>
-      </c>
-      <c r="O4" s="62">
+      <c r="N4" s="76">
+        <f>$B$16/M4</f>
+        <v>4.1499999999999995</v>
+      </c>
+      <c r="O4" s="92">
         <f>10000/N4</f>
-        <v>41500</v>
+        <v>2409.6385542168678</v>
       </c>
       <c r="P4" s="8">
-        <f>O4/$F$14 *100</f>
-        <v>415.00000000000006</v>
+        <f>O4/$F$14</f>
+        <v>0.24096385542168677</v>
       </c>
       <c r="Q4" s="42">
         <v>58.6</v>
       </c>
-      <c r="R4" s="8">
-        <f t="shared" si="0"/>
-        <v>58.6</v>
+      <c r="R4" s="73">
+        <f>$B$17/Q4</f>
+        <v>1.7064846416382253E-2</v>
       </c>
       <c r="S4" s="55" t="s">
         <v>0</v>
@@ -1428,61 +1437,61 @@
         <v>6052</v>
       </c>
       <c r="C5" s="5">
+        <f t="shared" si="0"/>
+        <v>0.94888679836939482</v>
+      </c>
+      <c r="D5" s="4">
         <f t="shared" si="1"/>
-        <v>0.94888679836939482</v>
-      </c>
-      <c r="D5" s="4">
+        <v>108</v>
+      </c>
+      <c r="E5" s="48">
         <f t="shared" si="2"/>
-        <v>108</v>
-      </c>
-      <c r="E5" s="48">
-        <f t="shared" si="3"/>
         <v>0.72240802675585281</v>
       </c>
-      <c r="F5" s="71" t="s">
+      <c r="F5" s="61" t="s">
         <v>22</v>
       </c>
       <c r="G5" s="4">
         <v>109</v>
       </c>
       <c r="H5" s="48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.72909698996655514</v>
       </c>
-      <c r="I5" s="71" t="s">
+      <c r="I5" s="61" t="s">
         <v>22</v>
       </c>
       <c r="J5" s="4">
         <v>107</v>
       </c>
       <c r="K5" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.71571906354515047</v>
       </c>
-      <c r="L5" s="71" t="s">
+      <c r="L5" s="61" t="s">
         <v>22</v>
       </c>
       <c r="M5" s="4">
         <v>224.7</v>
       </c>
-      <c r="N5" s="63">
-        <f t="shared" si="6"/>
+      <c r="N5" s="77">
+        <f t="shared" ref="N5:N12" si="5">$B$16/M5</f>
+        <v>1.6252781486426346</v>
+      </c>
+      <c r="O5" s="93">
+        <f>10000/N5</f>
+        <v>6152.7929901423877</v>
+      </c>
+      <c r="P5" s="5">
+        <f>O5/$F$14</f>
         <v>0.61527929901423872</v>
-      </c>
-      <c r="O5" s="64">
-        <f t="shared" ref="O5:O12" si="7">10000/N5</f>
-        <v>16252.781486426347</v>
-      </c>
-      <c r="P5" s="5">
-        <f t="shared" ref="P5:P12" si="8">O5/$F$14*100</f>
-        <v>162.52781486426346</v>
       </c>
       <c r="Q5" s="43">
         <v>241</v>
       </c>
-      <c r="R5" s="5">
-        <f t="shared" si="0"/>
-        <v>241</v>
+      <c r="R5" s="74">
+        <f>$B$17/Q5</f>
+        <v>4.1493775933609959E-3</v>
       </c>
       <c r="S5" s="56" t="s">
         <v>1</v>
@@ -1496,60 +1505,60 @@
         <v>6378</v>
       </c>
       <c r="C6" s="35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D6" s="36">
         <f t="shared" si="1"/>
+        <v>149.5</v>
+      </c>
+      <c r="E6" s="49">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="D6" s="36">
-        <f t="shared" si="2"/>
-        <v>149.5</v>
-      </c>
-      <c r="E6" s="49">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="F6" s="74" t="s">
+      <c r="F6" s="64" t="s">
         <v>22</v>
       </c>
       <c r="G6" s="33">
         <v>152</v>
       </c>
       <c r="H6" s="49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.0167224080267558</v>
       </c>
-      <c r="I6" s="74" t="s">
+      <c r="I6" s="64" t="s">
         <v>22</v>
       </c>
       <c r="J6" s="33">
         <v>147</v>
       </c>
       <c r="K6" s="49">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.98327759197324416</v>
       </c>
-      <c r="L6" s="74" t="s">
+      <c r="L6" s="64" t="s">
         <v>22</v>
       </c>
       <c r="M6" s="36">
         <v>365.2</v>
       </c>
-      <c r="N6" s="65">
-        <f t="shared" si="6"/>
+      <c r="N6" s="80">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="O6" s="66">
-        <f t="shared" si="7"/>
+      <c r="O6" s="94">
+        <f>10000/N6</f>
         <v>10000</v>
       </c>
       <c r="P6" s="35">
-        <f t="shared" si="8"/>
-        <v>100</v>
-      </c>
-      <c r="Q6" s="75">
+        <f>O6/$F$14</f>
         <v>1</v>
       </c>
-      <c r="R6" s="35">
-        <f>Q6/$B$17</f>
+      <c r="Q6" s="65">
+        <v>1</v>
+      </c>
+      <c r="R6" s="79">
+        <f t="shared" ref="R6:R12" si="6">$B$17/Q6</f>
         <v>1</v>
       </c>
       <c r="S6" s="57" t="s">
@@ -1564,61 +1573,61 @@
         <v>3396</v>
       </c>
       <c r="C7" s="5">
+        <f t="shared" si="0"/>
+        <v>0.53245531514581379</v>
+      </c>
+      <c r="D7" s="4">
         <f t="shared" si="1"/>
-        <v>0.53245531514581379</v>
-      </c>
-      <c r="D7" s="4">
+        <v>227</v>
+      </c>
+      <c r="E7" s="48">
         <f t="shared" si="2"/>
-        <v>227</v>
-      </c>
-      <c r="E7" s="48">
-        <f t="shared" si="3"/>
         <v>1.5183946488294315</v>
       </c>
-      <c r="F7" s="71" t="s">
+      <c r="F7" s="61" t="s">
         <v>22</v>
       </c>
       <c r="G7" s="4">
         <v>249</v>
       </c>
       <c r="H7" s="48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.6655518394648829</v>
       </c>
-      <c r="I7" s="71" t="s">
+      <c r="I7" s="61" t="s">
         <v>22</v>
       </c>
       <c r="J7" s="4">
         <v>205</v>
       </c>
       <c r="K7" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.3712374581939799</v>
       </c>
-      <c r="L7" s="71" t="s">
+      <c r="L7" s="61" t="s">
         <v>22</v>
       </c>
       <c r="M7" s="4">
         <v>687</v>
       </c>
-      <c r="N7" s="63">
-        <f t="shared" si="6"/>
-        <v>1.8811610076670318</v>
-      </c>
-      <c r="O7" s="64">
-        <f t="shared" si="7"/>
-        <v>5315.8660844250362</v>
+      <c r="N7" s="77">
+        <f t="shared" si="5"/>
+        <v>0.53158660844250361</v>
+      </c>
+      <c r="O7" s="93">
+        <f>10000/N7</f>
+        <v>18811.61007667032</v>
       </c>
       <c r="P7" s="5">
-        <f t="shared" si="8"/>
-        <v>53.158660844250363</v>
+        <f>O7/$F$14</f>
+        <v>1.881161007667032</v>
       </c>
       <c r="Q7" s="43">
         <v>1.03</v>
       </c>
-      <c r="R7" s="5">
-        <f t="shared" si="0"/>
-        <v>1.03</v>
+      <c r="R7" s="74">
+        <f t="shared" si="6"/>
+        <v>0.970873786407767</v>
       </c>
       <c r="S7" s="56" t="s">
         <v>3</v>
@@ -1632,15 +1641,15 @@
         <v>71492</v>
       </c>
       <c r="C8" s="5">
+        <f t="shared" si="0"/>
+        <v>11.209156475384132</v>
+      </c>
+      <c r="D8" s="4">
         <f t="shared" si="1"/>
-        <v>11.209156475384132</v>
-      </c>
-      <c r="D8" s="4">
+        <v>779</v>
+      </c>
+      <c r="E8" s="48">
         <f t="shared" si="2"/>
-        <v>779</v>
-      </c>
-      <c r="E8" s="48">
-        <f t="shared" si="3"/>
         <v>5.2107023411371234</v>
       </c>
       <c r="F8" s="5">
@@ -1651,7 +1660,7 @@
         <v>817</v>
       </c>
       <c r="H8" s="48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>5.4648829431438131</v>
       </c>
       <c r="I8" s="5">
@@ -1662,7 +1671,7 @@
         <v>741</v>
       </c>
       <c r="K8" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.9565217391304346</v>
       </c>
       <c r="L8" s="5">
@@ -1672,24 +1681,24 @@
       <c r="M8" s="4">
         <v>4332</v>
       </c>
-      <c r="N8" s="63">
-        <f t="shared" si="6"/>
+      <c r="N8" s="77">
+        <f t="shared" si="5"/>
+        <v>8.4302862419205912E-2</v>
+      </c>
+      <c r="O8" s="93">
+        <f>10000/N8</f>
+        <v>118619.93428258489</v>
+      </c>
+      <c r="P8" s="5">
+        <f>O8/$F$14</f>
         <v>11.861993428258488</v>
-      </c>
-      <c r="O8" s="64">
-        <f t="shared" si="7"/>
-        <v>843.02862419205917</v>
-      </c>
-      <c r="P8" s="5">
-        <f t="shared" si="8"/>
-        <v>8.4302862419205908</v>
       </c>
       <c r="Q8" s="43">
         <v>0.40899999999999997</v>
       </c>
-      <c r="R8" s="5">
-        <f t="shared" si="0"/>
-        <v>0.40899999999999997</v>
+      <c r="R8" s="74">
+        <f t="shared" si="6"/>
+        <v>2.4449877750611249</v>
       </c>
       <c r="S8" s="56" t="s">
         <v>4</v>
@@ -1703,15 +1712,15 @@
         <v>60268</v>
       </c>
       <c r="C9" s="5">
+        <f t="shared" si="0"/>
+        <v>9.4493571652555666</v>
+      </c>
+      <c r="D9" s="4">
         <f t="shared" si="1"/>
-        <v>9.4493571652555666</v>
-      </c>
-      <c r="D9" s="4">
+        <v>1430</v>
+      </c>
+      <c r="E9" s="48">
         <f t="shared" si="2"/>
-        <v>1430</v>
-      </c>
-      <c r="E9" s="48">
-        <f t="shared" si="3"/>
         <v>9.5652173913043477</v>
       </c>
       <c r="F9" s="5">
@@ -1722,7 +1731,7 @@
         <v>1510</v>
       </c>
       <c r="H9" s="48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>10.100334448160535</v>
       </c>
       <c r="I9" s="5">
@@ -1733,7 +1742,7 @@
         <v>1350</v>
       </c>
       <c r="K9" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>9.0301003344481607</v>
       </c>
       <c r="L9" s="5">
@@ -1743,24 +1752,24 @@
       <c r="M9" s="4">
         <v>10760</v>
       </c>
-      <c r="N9" s="63">
-        <f t="shared" si="6"/>
-        <v>29.463307776560789</v>
-      </c>
-      <c r="O9" s="64">
-        <f t="shared" si="7"/>
-        <v>339.40520446096656</v>
+      <c r="N9" s="77">
+        <f t="shared" si="5"/>
+        <v>3.3940520446096654E-2</v>
+      </c>
+      <c r="O9" s="93">
+        <f>10000/N9</f>
+        <v>294633.07776560786</v>
       </c>
       <c r="P9" s="5">
-        <f t="shared" si="8"/>
-        <v>3.3940520446096656</v>
+        <f>O9/$F$14</f>
+        <v>29.463307776560786</v>
       </c>
       <c r="Q9" s="43">
         <v>0.438</v>
       </c>
-      <c r="R9" s="5">
-        <f t="shared" si="0"/>
-        <v>0.438</v>
+      <c r="R9" s="74">
+        <f t="shared" si="6"/>
+        <v>2.2831050228310503</v>
       </c>
       <c r="S9" s="56" t="s">
         <v>5</v>
@@ -1774,15 +1783,15 @@
         <v>25559</v>
       </c>
       <c r="C10" s="5">
+        <f t="shared" si="0"/>
+        <v>4.007369081216682</v>
+      </c>
+      <c r="D10" s="4">
         <f t="shared" si="1"/>
-        <v>4.007369081216682</v>
-      </c>
-      <c r="D10" s="4">
+        <v>2875</v>
+      </c>
+      <c r="E10" s="48">
         <f t="shared" si="2"/>
-        <v>2875</v>
-      </c>
-      <c r="E10" s="48">
-        <f t="shared" si="3"/>
         <v>19.23076923076923</v>
       </c>
       <c r="F10" s="5">
@@ -1793,7 +1802,7 @@
         <v>3000</v>
       </c>
       <c r="H10" s="48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>20.066889632107024</v>
       </c>
       <c r="I10" s="5">
@@ -1804,7 +1813,7 @@
         <v>2750</v>
       </c>
       <c r="K10" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>18.394648829431439</v>
       </c>
       <c r="L10" s="5">
@@ -1814,24 +1823,24 @@
       <c r="M10" s="4">
         <v>30700</v>
       </c>
-      <c r="N10" s="63">
-        <f t="shared" si="6"/>
+      <c r="N10" s="77">
+        <f t="shared" si="5"/>
+        <v>1.1895765472312704E-2</v>
+      </c>
+      <c r="O10" s="93">
+        <f>10000/N10</f>
+        <v>840635.26834611176</v>
+      </c>
+      <c r="P10" s="5">
+        <f>O10/$F$14</f>
         <v>84.063526834611181</v>
-      </c>
-      <c r="O10" s="64">
-        <f t="shared" si="7"/>
-        <v>118.95765472312702</v>
-      </c>
-      <c r="P10" s="5">
-        <f t="shared" si="8"/>
-        <v>1.1895765472312703</v>
       </c>
       <c r="Q10" s="43">
         <v>0.75</v>
       </c>
-      <c r="R10" s="5">
-        <f t="shared" si="0"/>
-        <v>0.75</v>
+      <c r="R10" s="74">
+        <f t="shared" si="6"/>
+        <v>1.3333333333333333</v>
       </c>
       <c r="S10" s="56" t="s">
         <v>6</v>
@@ -1845,15 +1854,15 @@
         <v>24764</v>
       </c>
       <c r="C11" s="5">
+        <f t="shared" si="0"/>
+        <v>3.8827218563813108</v>
+      </c>
+      <c r="D11" s="4">
         <f t="shared" si="1"/>
-        <v>3.8827218563813108</v>
-      </c>
-      <c r="D11" s="4">
+        <v>4500</v>
+      </c>
+      <c r="E11" s="48">
         <f t="shared" si="2"/>
-        <v>4500</v>
-      </c>
-      <c r="E11" s="48">
-        <f t="shared" si="3"/>
         <v>30.100334448160535</v>
       </c>
       <c r="F11" s="5">
@@ -1864,7 +1873,7 @@
         <v>4550</v>
       </c>
       <c r="H11" s="48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>30.434782608695652</v>
       </c>
       <c r="I11" s="5">
@@ -1875,7 +1884,7 @@
         <v>4450</v>
       </c>
       <c r="K11" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>29.765886287625417</v>
       </c>
       <c r="L11" s="5">
@@ -1885,24 +1894,24 @@
       <c r="M11" s="4">
         <v>60200</v>
       </c>
-      <c r="N11" s="63">
-        <f t="shared" si="6"/>
+      <c r="N11" s="77">
+        <f t="shared" si="5"/>
+        <v>6.0664451827242526E-3</v>
+      </c>
+      <c r="O11" s="93">
+        <f>10000/N11</f>
+        <v>1648411.8291347206</v>
+      </c>
+      <c r="P11" s="5">
+        <f>O11/$F$14</f>
         <v>164.84118291347207</v>
-      </c>
-      <c r="O11" s="64">
-        <f t="shared" si="7"/>
-        <v>60.664451827242523</v>
-      </c>
-      <c r="P11" s="5">
-        <f t="shared" si="8"/>
-        <v>0.60664451827242527</v>
       </c>
       <c r="Q11" s="43">
         <v>0.79</v>
       </c>
-      <c r="R11" s="5">
-        <f t="shared" si="0"/>
-        <v>0.79</v>
+      <c r="R11" s="74">
+        <f t="shared" si="6"/>
+        <v>1.2658227848101264</v>
       </c>
       <c r="S11" s="56" t="s">
         <v>7</v>
@@ -1916,15 +1925,15 @@
         <v>2302</v>
       </c>
       <c r="C12" s="7">
+        <f t="shared" si="0"/>
+        <v>0.36092819065537785</v>
+      </c>
+      <c r="D12" s="6">
         <f t="shared" si="1"/>
-        <v>0.36092819065537785</v>
-      </c>
-      <c r="D12" s="6">
+        <v>5910</v>
+      </c>
+      <c r="E12" s="50">
         <f t="shared" si="2"/>
-        <v>5910</v>
-      </c>
-      <c r="E12" s="50">
-        <f t="shared" si="3"/>
         <v>39.531772575250834</v>
       </c>
       <c r="F12" s="7">
@@ -1935,7 +1944,7 @@
         <v>7380</v>
       </c>
       <c r="H12" s="50">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>49.364548494983275</v>
       </c>
       <c r="I12" s="7">
@@ -1946,7 +1955,7 @@
         <v>4440</v>
       </c>
       <c r="K12" s="50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>29.698996655518396</v>
       </c>
       <c r="L12" s="7">
@@ -1956,24 +1965,24 @@
       <c r="M12" s="6">
         <v>90600</v>
       </c>
-      <c r="N12" s="67">
-        <f t="shared" si="6"/>
+      <c r="N12" s="78">
+        <f t="shared" si="5"/>
+        <v>4.0309050772626932E-3</v>
+      </c>
+      <c r="O12" s="95">
+        <f>10000/N12</f>
+        <v>2480832.4205914568</v>
+      </c>
+      <c r="P12" s="7">
+        <f>O12/$F$14</f>
         <v>248.08324205914568</v>
-      </c>
-      <c r="O12" s="68">
-        <f t="shared" si="7"/>
-        <v>40.309050772626932</v>
-      </c>
-      <c r="P12" s="7">
-        <f t="shared" si="8"/>
-        <v>0.40309050772626931</v>
       </c>
       <c r="Q12" s="44">
         <v>6.4</v>
       </c>
-      <c r="R12" s="7">
-        <f t="shared" si="0"/>
-        <v>6.4</v>
+      <c r="R12" s="75">
+        <f t="shared" si="6"/>
+        <v>0.15625</v>
       </c>
       <c r="S12" s="58" t="s">
         <v>8</v>
@@ -1989,22 +1998,22 @@
         <v>149.5</v>
       </c>
       <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="89" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="89"/>
-      <c r="F14" s="76">
+      <c r="E14" s="67"/>
+      <c r="F14" s="66">
         <f>O6</f>
         <v>10000</v>
       </c>
-      <c r="H14" s="83" t="s">
+      <c r="H14" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="I14" s="83"/>
-      <c r="J14" s="83"/>
-      <c r="K14" s="83"/>
+      <c r="I14" s="71"/>
+      <c r="J14" s="71"/>
+      <c r="K14" s="71"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="38" t="s">
@@ -2017,19 +2026,19 @@
       <c r="C15" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="77" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" s="77"/>
+      <c r="D15" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="68"/>
       <c r="F15" s="1">
         <v>100</v>
       </c>
-      <c r="H15" s="83" t="s">
+      <c r="H15" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="I15" s="83"/>
-      <c r="J15" s="83"/>
-      <c r="K15" s="83"/>
+      <c r="I15" s="71"/>
+      <c r="J15" s="71"/>
+      <c r="K15" s="71"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="38" t="s">
@@ -2045,12 +2054,12 @@
       <c r="F16" s="1">
         <v>240</v>
       </c>
-      <c r="H16" s="83" t="s">
+      <c r="H16" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="I16" s="83"/>
-      <c r="J16" s="83"/>
-      <c r="K16" s="83"/>
+      <c r="I16" s="71"/>
+      <c r="J16" s="71"/>
+      <c r="K16" s="71"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="38" t="s">
@@ -2063,12 +2072,12 @@
       <c r="C17" t="s">
         <v>32</v>
       </c>
-      <c r="H17" s="83" t="s">
+      <c r="H17" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="I17" s="83"/>
-      <c r="J17" s="83"/>
-      <c r="K17" s="83"/>
+      <c r="I17" s="71"/>
+      <c r="J17" s="71"/>
+      <c r="K17" s="71"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="30"/>
@@ -2105,11 +2114,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="D14:E14"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="O2:P2"/>
@@ -2118,6 +2122,11 @@
     <mergeCell ref="H16:K16"/>
     <mergeCell ref="H15:K15"/>
     <mergeCell ref="H14:K14"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="D14:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="45" orientation="portrait" r:id="rId1"/>

</xml_diff>